<commit_message>
finalised test results for user acceptance test
</commit_message>
<xml_diff>
--- a/00. Testing/00. Documentation/03. Test Execution & Results/Test Execution and Results V2 Results Inputted.xlsx
+++ b/00. Testing/00. Documentation/03. Test Execution & Results/Test Execution and Results V2 Results Inputted.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roqit-my.sharepoint.com/personal/james_croxford_roq_co_uk/Documents/Documents/05. Repos/01. Bootcamp/Final Showcase/CredersiVendAdmin/00. Testing/00. Documentation/03. Test Execution &amp; Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roqit-my.sharepoint.com/personal/avais_hussain_roq_co_uk/Documents/Desktop/GroupProject/CredersiVendAdmin/00. Testing/00. Documentation/03. Test Execution &amp; Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="257" documentId="8_{A80CC677-47EF-45E4-BCD1-DBCDF5E6E5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0737B7E5-7BC7-4A7F-9822-F7CA321D08E5}"/>
+  <xr:revisionPtr revIDLastSave="362" documentId="8_{A80CC677-47EF-45E4-BCD1-DBCDF5E6E5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11C715BF-3BEE-4872-B32C-B5AD0AC8A4BC}"/>
   <bookViews>
-    <workbookView xWindow="32220" yWindow="825" windowWidth="25380" windowHeight="11880" activeTab="1" xr2:uid="{40B22CA0-7C7F-4DF3-AD4C-55C353439023}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{40B22CA0-7C7F-4DF3-AD4C-55C353439023}"/>
   </bookViews>
   <sheets>
     <sheet name="User Acceptance" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="446">
   <si>
     <t>Automated User Acceptance Tests Cases</t>
   </si>
@@ -1727,6 +1727,45 @@
   </si>
   <si>
     <t>Despite user work around to log out of admin account, still have visibile access to data that should only be viewable when logged in. To fully 'log out' user has to also refresh the page. User can use browser back button to cycle through UUIDs in address bar for various components. May present data breach issue. Hard to determine without full site features and implementation.</t>
+  </si>
+  <si>
+    <t>No warning/restriction. System allows user to load onto the application and find the title when it has been displayed.</t>
+  </si>
+  <si>
+    <t>No warning/restriction. The webpage loads for the user and found a login button on the application</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>No warning/restriction. The webpage loads for the user and found the username box</t>
+  </si>
+  <si>
+    <t>No warning/restriction. The webpage loads for the user and found the password box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No warning/restriction. The webpage loads for the user and has a login button </t>
+  </si>
+  <si>
+    <t>No warning/restriction. The webpage loads for the user and found the username label</t>
+  </si>
+  <si>
+    <t>No warning/restriction. The webpage loads for the user and found the password label</t>
+  </si>
+  <si>
+    <t>No warning/restriction. The webpage logo from the login page loads and is visible.</t>
+  </si>
+  <si>
+    <t>No warning/restriction. The webpage loads for the user and found the element for the username text exist</t>
+  </si>
+  <si>
+    <t>No warning/restriction. The webpage loads for the user and found the element for the password text exist</t>
+  </si>
+  <si>
+    <t>No warning/ restriction. System allow user to load to the log in page. It loads the user in and allows the user to create a new customer and is displyed on the customer page.</t>
+  </si>
+  <si>
+    <t>No issue noted Test case passed</t>
   </si>
 </sst>
 </file>
@@ -2050,7 +2089,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2140,11 +2179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2204,37 +2239,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="105">
-    <dxf>
+  <dxfs count="109">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2260,11 +2286,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2280,11 +2306,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2300,11 +2326,32 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2319,13 +2366,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -2337,6 +2377,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2346,14 +2396,61 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -2365,6 +2462,40 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2381,129 +2512,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2776,6 +2784,25 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3046,6 +3073,25 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -3322,6 +3368,25 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3610,6 +3675,25 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -3852,84 +3936,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{999B60BA-87BB-4384-9F87-F39587B5D78C}" name="Table1" displayName="Table1" ref="A5:M37" totalsRowShown="0" headerRowDxfId="104" dataDxfId="102" headerRowBorderDxfId="103" tableBorderDxfId="101" totalsRowBorderDxfId="100" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{999B60BA-87BB-4384-9F87-F39587B5D78C}" name="Table1" displayName="Table1" ref="A5:M37" totalsRowShown="0" headerRowDxfId="108" dataDxfId="106" headerRowBorderDxfId="107" tableBorderDxfId="105" totalsRowBorderDxfId="104" headerRowCellStyle="Heading 1">
   <autoFilter ref="A5:M37" xr:uid="{999B60BA-87BB-4384-9F87-F39587B5D78C}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{3AF0BC11-7411-4ED3-8FE2-283F407B9F63}" name="Test ID" dataDxfId="99"/>
-    <tableColumn id="12" xr3:uid="{5E16E47E-778B-4087-BE9F-FAC69BBFBFD7}" name="Test Case" dataDxfId="98"/>
-    <tableColumn id="4" xr3:uid="{C1771649-7AEE-4C22-ABD2-4A7A5D683F41}" name="Functional Area" dataDxfId="97"/>
-    <tableColumn id="6" xr3:uid="{716C132F-79C8-4367-8E9B-23FB0286A718}" name="Test Steps" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{99BBD767-6BE6-4E1B-8348-55530618901B}" name="Test Tool" dataDxfId="95"/>
-    <tableColumn id="13" xr3:uid="{CAFBA488-3AC0-40BA-A7DF-643DA9826A91}" name="Test Dependencies" dataDxfId="94"/>
-    <tableColumn id="7" xr3:uid="{33561203-36C8-4596-89EF-29D55DF6BCC8}" name="Test Data" dataDxfId="93"/>
-    <tableColumn id="8" xr3:uid="{3AB831DC-E315-4439-8ACE-8DAC9BB2375D}" name="Expected Outcome" dataDxfId="92"/>
-    <tableColumn id="14" xr3:uid="{1DCB53BF-9FB4-4BE8-9F51-ABE096FA7E26}" name="Tester" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{D427E3E6-B93E-496C-9D8D-5362CFA48EA1}" name="Actual Outcome" dataDxfId="91"/>
-    <tableColumn id="10" xr3:uid="{25206BA6-07F1-41D8-AD0A-D238F20DF1E5}" name="PASS/FAIL" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{45C75F4A-F282-48C5-8652-CC9CB1B0F6A6}" name="Defect Report ID" dataDxfId="89"/>
-    <tableColumn id="11" xr3:uid="{29AF0B64-26AE-4BC5-9992-49F9E00D7CC1}" name="Conclusion" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{3AF0BC11-7411-4ED3-8FE2-283F407B9F63}" name="Test ID" dataDxfId="103"/>
+    <tableColumn id="12" xr3:uid="{5E16E47E-778B-4087-BE9F-FAC69BBFBFD7}" name="Test Case" dataDxfId="102"/>
+    <tableColumn id="4" xr3:uid="{C1771649-7AEE-4C22-ABD2-4A7A5D683F41}" name="Functional Area" dataDxfId="101"/>
+    <tableColumn id="6" xr3:uid="{716C132F-79C8-4367-8E9B-23FB0286A718}" name="Test Steps" dataDxfId="100"/>
+    <tableColumn id="5" xr3:uid="{99BBD767-6BE6-4E1B-8348-55530618901B}" name="Test Tool" dataDxfId="99"/>
+    <tableColumn id="13" xr3:uid="{CAFBA488-3AC0-40BA-A7DF-643DA9826A91}" name="Test Dependencies" dataDxfId="98"/>
+    <tableColumn id="7" xr3:uid="{33561203-36C8-4596-89EF-29D55DF6BCC8}" name="Test Data" dataDxfId="97"/>
+    <tableColumn id="8" xr3:uid="{3AB831DC-E315-4439-8ACE-8DAC9BB2375D}" name="Expected Outcome" dataDxfId="96"/>
+    <tableColumn id="14" xr3:uid="{1DCB53BF-9FB4-4BE8-9F51-ABE096FA7E26}" name="Tester" dataDxfId="95"/>
+    <tableColumn id="9" xr3:uid="{D427E3E6-B93E-496C-9D8D-5362CFA48EA1}" name="Actual Outcome" dataDxfId="94"/>
+    <tableColumn id="10" xr3:uid="{25206BA6-07F1-41D8-AD0A-D238F20DF1E5}" name="PASS/FAIL" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{45C75F4A-F282-48C5-8652-CC9CB1B0F6A6}" name="Defect Report ID" dataDxfId="92"/>
+    <tableColumn id="11" xr3:uid="{29AF0B64-26AE-4BC5-9992-49F9E00D7CC1}" name="Conclusion" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81DD9B57-FC13-4A2B-A043-0981C373D135}" name="Table2" displayName="Table2" ref="A5:M37" totalsRowShown="0" headerRowDxfId="87" dataDxfId="85" headerRowBorderDxfId="86" tableBorderDxfId="84" totalsRowBorderDxfId="83" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81DD9B57-FC13-4A2B-A043-0981C373D135}" name="Table2" displayName="Table2" ref="A5:M37" totalsRowShown="0" headerRowDxfId="90" dataDxfId="88" headerRowBorderDxfId="89" tableBorderDxfId="87" totalsRowBorderDxfId="86" headerRowCellStyle="Heading 1">
   <autoFilter ref="A5:M37" xr:uid="{81DD9B57-FC13-4A2B-A043-0981C373D135}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{DDD3F64F-F3BA-4CA1-AC99-E6A91F7EFB2A}" name="Test ID" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{3651F69B-7632-4BBF-928B-D714EAFF8112}" name="Test Case" dataDxfId="81"/>
-    <tableColumn id="5" xr3:uid="{95E485BF-6025-49F0-8195-4CC41A3D488B}" name="Functional Area" dataDxfId="80"/>
-    <tableColumn id="6" xr3:uid="{CB5E0D49-9E8A-4FA8-AB2E-E92F4EFA1344}" name="Test Steps" dataDxfId="79"/>
-    <tableColumn id="7" xr3:uid="{9D0EDB81-502A-4D1F-B86B-A37934B87143}" name="Test Tool" dataDxfId="78"/>
-    <tableColumn id="8" xr3:uid="{E04F1A31-A155-4ED0-8CC8-51DA1416E22B}" name="Test Dependencies" dataDxfId="77"/>
-    <tableColumn id="9" xr3:uid="{FA1C7AF5-453A-4B4A-8EA7-F8E2C46830C9}" name="Test Data" dataDxfId="76"/>
-    <tableColumn id="10" xr3:uid="{39C87776-74B4-4F3B-BBA7-C5C745411551}" name="Expected Outcome" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{B954A7BB-9475-4833-B6AD-4DC432CFE894}" name="Tester" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{579A88E4-258E-46F2-999A-7D5703CB0D43}" name="Actual Outcome" dataDxfId="74"/>
-    <tableColumn id="12" xr3:uid="{7DA60FF0-EBC8-4FE0-B513-8457A780F171}" name="PASS/FAIL" dataDxfId="73"/>
-    <tableColumn id="16" xr3:uid="{902DB2B5-1EE5-42AD-8D4B-48B8314F088B}" name="Defect Report ID" dataDxfId="72"/>
-    <tableColumn id="14" xr3:uid="{D0C57132-3E48-4444-A1FD-F203D0455563}" name="Conclusion" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{DDD3F64F-F3BA-4CA1-AC99-E6A91F7EFB2A}" name="Test ID" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{3651F69B-7632-4BBF-928B-D714EAFF8112}" name="Test Case" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{95E485BF-6025-49F0-8195-4CC41A3D488B}" name="Functional Area" dataDxfId="83"/>
+    <tableColumn id="6" xr3:uid="{CB5E0D49-9E8A-4FA8-AB2E-E92F4EFA1344}" name="Test Steps" dataDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{9D0EDB81-502A-4D1F-B86B-A37934B87143}" name="Test Tool" dataDxfId="81"/>
+    <tableColumn id="8" xr3:uid="{E04F1A31-A155-4ED0-8CC8-51DA1416E22B}" name="Test Dependencies" dataDxfId="80"/>
+    <tableColumn id="9" xr3:uid="{FA1C7AF5-453A-4B4A-8EA7-F8E2C46830C9}" name="Test Data" dataDxfId="79"/>
+    <tableColumn id="10" xr3:uid="{39C87776-74B4-4F3B-BBA7-C5C745411551}" name="Expected Outcome" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{B954A7BB-9475-4833-B6AD-4DC432CFE894}" name="Tester" dataDxfId="77"/>
+    <tableColumn id="11" xr3:uid="{579A88E4-258E-46F2-999A-7D5703CB0D43}" name="Actual Outcome" dataDxfId="76"/>
+    <tableColumn id="12" xr3:uid="{7DA60FF0-EBC8-4FE0-B513-8457A780F171}" name="PASS/FAIL" dataDxfId="75"/>
+    <tableColumn id="16" xr3:uid="{902DB2B5-1EE5-42AD-8D4B-48B8314F088B}" name="Defect Report ID" dataDxfId="74"/>
+    <tableColumn id="14" xr3:uid="{D0C57132-3E48-4444-A1FD-F203D0455563}" name="Conclusion" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4CF6D82A-905D-4759-B510-EB45783C3273}" name="Table8" displayName="Table8" ref="A42:M64" totalsRowShown="0" headerRowDxfId="70" dataDxfId="68" headerRowBorderDxfId="69" tableBorderDxfId="67" totalsRowBorderDxfId="66" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4CF6D82A-905D-4759-B510-EB45783C3273}" name="Table8" displayName="Table8" ref="A42:M64" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69" totalsRowBorderDxfId="68" headerRowCellStyle="Heading 1">
   <autoFilter ref="A42:M64" xr:uid="{4CF6D82A-905D-4759-B510-EB45783C3273}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{BC6B0D91-86AC-473C-888D-76843E0F1E31}" name="Test ID" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{06E609F9-488D-426D-A10E-891E1ADB14C7}" name="Test Case" dataDxfId="64"/>
-    <tableColumn id="5" xr3:uid="{2ED639BC-7DC0-420A-9186-DFF942691ABA}" name="Functional Area" dataDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{6E2C3CB2-02A3-48FE-B7FB-DAFA0B0AB145}" name="Test Steps" dataDxfId="62"/>
-    <tableColumn id="7" xr3:uid="{35987979-9F3E-4ACD-AE5E-E56B5A848CB9}" name="Test Tool" dataDxfId="61"/>
-    <tableColumn id="8" xr3:uid="{0141D090-E639-49E8-9F28-C5AB63D0BC46}" name="Test Dependencies" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{B30019E5-BFA9-4BDB-B63C-F79D05457C9E}" name="Test Data" dataDxfId="59"/>
-    <tableColumn id="10" xr3:uid="{548855A0-DEA5-4405-B71F-2F2D86C3287E}" name="Expected Outcome" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{10808AC8-D54B-4AF5-8E02-3346890F0452}" name="Tester" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{CB9CFD07-1E2C-4B27-B39C-9C1EA3113E94}" name="Actual Outcome" dataDxfId="57"/>
-    <tableColumn id="12" xr3:uid="{2766A871-A298-4F79-833D-76D02D89B670}" name="PASS/FAIL" dataDxfId="56"/>
-    <tableColumn id="14" xr3:uid="{D161C0B0-0EB3-4F71-AF42-C0D8C5317688}" name="Defect Report ID" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{ED9D2976-6B15-4485-AC03-64BAB821A836}" name="Conclusion" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{BC6B0D91-86AC-473C-888D-76843E0F1E31}" name="Test ID" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{06E609F9-488D-426D-A10E-891E1ADB14C7}" name="Test Case" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{2ED639BC-7DC0-420A-9186-DFF942691ABA}" name="Functional Area" dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{6E2C3CB2-02A3-48FE-B7FB-DAFA0B0AB145}" name="Test Steps" dataDxfId="64"/>
+    <tableColumn id="7" xr3:uid="{35987979-9F3E-4ACD-AE5E-E56B5A848CB9}" name="Test Tool" dataDxfId="63"/>
+    <tableColumn id="8" xr3:uid="{0141D090-E639-49E8-9F28-C5AB63D0BC46}" name="Test Dependencies" dataDxfId="62"/>
+    <tableColumn id="9" xr3:uid="{B30019E5-BFA9-4BDB-B63C-F79D05457C9E}" name="Test Data" dataDxfId="61"/>
+    <tableColumn id="10" xr3:uid="{548855A0-DEA5-4405-B71F-2F2D86C3287E}" name="Expected Outcome" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{10808AC8-D54B-4AF5-8E02-3346890F0452}" name="Tester" dataDxfId="59"/>
+    <tableColumn id="11" xr3:uid="{CB9CFD07-1E2C-4B27-B39C-9C1EA3113E94}" name="Actual Outcome" dataDxfId="58"/>
+    <tableColumn id="12" xr3:uid="{2766A871-A298-4F79-833D-76D02D89B670}" name="PASS/FAIL" dataDxfId="57"/>
+    <tableColumn id="14" xr3:uid="{D161C0B0-0EB3-4F71-AF42-C0D8C5317688}" name="Defect Report ID" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{ED9D2976-6B15-4485-AC03-64BAB821A836}" name="Conclusion" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{63F8CF34-8D5D-41C8-8C79-6F61B7AA084A}" name="Table3" displayName="Table3" ref="A4:M17" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" totalsRowBorderDxfId="49" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{63F8CF34-8D5D-41C8-8C79-6F61B7AA084A}" name="Table3" displayName="Table3" ref="A4:M17" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50" headerRowCellStyle="Heading 1">
   <autoFilter ref="A4:M17" xr:uid="{63F8CF34-8D5D-41C8-8C79-6F61B7AA084A}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{5FD902D6-F8D8-400F-BBE3-0450997CF60F}" name="Test ID" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{10EAD06E-09FD-4032-9756-4C551FCCEE2A}" name="Test Case" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{BA02662A-1E44-467D-852F-A05C4C958DBD}" name="Notes" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{83CB7963-B21D-4965-AF7A-BB02268C112D}" name="Test Steps" dataDxfId="45"/>
-    <tableColumn id="7" xr3:uid="{189B9710-382A-40AE-B1FD-A8B78369467A}" name="Test Tool" dataDxfId="44"/>
-    <tableColumn id="8" xr3:uid="{CB1B2D16-4FB2-4E23-BAB2-1FA0FB6BF1BD}" name="Test Dependencies" dataDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{05982C6D-7240-443D-B3E1-CF9667A784CF}" name="Test Data" dataDxfId="42"/>
-    <tableColumn id="10" xr3:uid="{2831798C-2F4C-4F6D-8D97-9902DC545376}" name="Expected Outcome" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{F270A6EF-DB2F-487E-A422-63BDF33EB05C}" name="Tester" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{5FD902D6-F8D8-400F-BBE3-0450997CF60F}" name="Test ID" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{10EAD06E-09FD-4032-9756-4C551FCCEE2A}" name="Test Case" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{BA02662A-1E44-467D-852F-A05C4C958DBD}" name="Notes" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{83CB7963-B21D-4965-AF7A-BB02268C112D}" name="Test Steps" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{189B9710-382A-40AE-B1FD-A8B78369467A}" name="Test Tool" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{CB1B2D16-4FB2-4E23-BAB2-1FA0FB6BF1BD}" name="Test Dependencies" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{05982C6D-7240-443D-B3E1-CF9667A784CF}" name="Test Data" dataDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{2831798C-2F4C-4F6D-8D97-9902DC545376}" name="Expected Outcome" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{F270A6EF-DB2F-487E-A422-63BDF33EB05C}" name="Tester" dataDxfId="41"/>
     <tableColumn id="11" xr3:uid="{B5BDCB48-F450-4E21-BC57-A360D2F2DF09}" name="Actual Outcome" dataDxfId="40"/>
     <tableColumn id="12" xr3:uid="{D3A73122-07BD-41C4-9D0D-A48FC26EFC0A}" name="PASS/FAIL" dataDxfId="39"/>
     <tableColumn id="13" xr3:uid="{D93B5FBA-D33D-4DF2-B318-AAF70A375F25}" name="Defect Report ID" dataDxfId="38"/>
@@ -3951,11 +4035,11 @@
     <tableColumn id="8" xr3:uid="{23AA4EBA-6F6C-4784-804A-7E2349416FC2}" name="Test Dependencies" dataDxfId="26"/>
     <tableColumn id="9" xr3:uid="{0C5FD806-3ED1-46A4-9BC2-CA0D7D3FA68F}" name="Test Data" dataDxfId="25"/>
     <tableColumn id="10" xr3:uid="{016CAF80-79FF-4D02-944B-72954947E84F}" name="Expected Outcome" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{B890E844-FC0D-42C1-A845-1AB9E326AAA5}" name="Tester" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{5CE96462-FB7C-4C17-8481-AE021B661191}" name="Actual Outcome" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{E0B5B100-9D58-4515-85A5-1F2F737E5828}" name="PASS/FAIL" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{41D2F203-BBEF-4567-8881-C39A8D70DE49}" name="Defect Report ID" dataDxfId="21"/>
-    <tableColumn id="13" xr3:uid="{58E6A6BA-BDD0-4A2F-801E-A4AE3AB1465B}" name="Conclusion" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{B890E844-FC0D-42C1-A845-1AB9E326AAA5}" name="Tester" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{5CE96462-FB7C-4C17-8481-AE021B661191}" name="Actual Outcome" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{E0B5B100-9D58-4515-85A5-1F2F737E5828}" name="PASS/FAIL" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{41D2F203-BBEF-4567-8881-C39A8D70DE49}" name="Defect Report ID" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{58E6A6BA-BDD0-4A2F-801E-A4AE3AB1465B}" name="Conclusion" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4260,44 +4344,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFED341-A0C6-4063-911E-0361A937A64A}">
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView topLeftCell="C30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="11" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="11" width="17.6640625" customWidth="1"/>
+    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="39" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="41"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-    </row>
-    <row r="5" spans="1:13" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="42"/>
+    </row>
+    <row r="5" spans="1:13" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -4330,14 +4414,14 @@
       <c r="K5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="37" t="s">
+      <c r="L5" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="M5" s="37" t="s">
+      <c r="M5" s="35" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>12</v>
       </c>
@@ -4365,12 +4449,18 @@
       <c r="I6" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="27"/>
-    </row>
-    <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="J6" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="K6" s="51" t="s">
+        <v>435</v>
+      </c>
+      <c r="L6" s="32"/>
+      <c r="M6" s="27" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>20</v>
       </c>
@@ -4398,12 +4488,18 @@
       <c r="I7" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="27"/>
-    </row>
-    <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="J7" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="K7" s="51" t="s">
+        <v>435</v>
+      </c>
+      <c r="L7" s="33"/>
+      <c r="M7" s="27" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>25</v>
       </c>
@@ -4431,12 +4527,18 @@
       <c r="I8" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="27"/>
-    </row>
-    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="J8" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="K8" s="51" t="s">
+        <v>435</v>
+      </c>
+      <c r="L8" s="32"/>
+      <c r="M8" s="27" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>30</v>
       </c>
@@ -4464,12 +4566,18 @@
       <c r="I9" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="27"/>
-    </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="J9" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="K9" s="51" t="s">
+        <v>435</v>
+      </c>
+      <c r="L9" s="32"/>
+      <c r="M9" s="27" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>35</v>
       </c>
@@ -4497,12 +4605,18 @@
       <c r="I10" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="27"/>
-    </row>
-    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="J10" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="L10" s="33"/>
+      <c r="M10" s="27" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>39</v>
       </c>
@@ -4530,12 +4644,18 @@
       <c r="I11" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="27"/>
-    </row>
-    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="J11" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="L11" s="33"/>
+      <c r="M11" s="27" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>43</v>
       </c>
@@ -4563,12 +4683,18 @@
       <c r="I12" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="27"/>
-    </row>
-    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="J12" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="K12" s="51" t="s">
+        <v>435</v>
+      </c>
+      <c r="L12" s="52"/>
+      <c r="M12" s="27" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>47</v>
       </c>
@@ -4596,12 +4722,18 @@
       <c r="I13" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="27"/>
-    </row>
-    <row r="14" spans="1:13" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="J13" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="K13" s="51" t="s">
+        <v>435</v>
+      </c>
+      <c r="L13" s="32"/>
+      <c r="M13" s="27" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="12" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>51</v>
       </c>
@@ -4629,12 +4761,18 @@
       <c r="I14" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="27"/>
-    </row>
-    <row r="15" spans="1:13" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="J14" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="K14" s="51" t="s">
+        <v>435</v>
+      </c>
+      <c r="L14" s="32"/>
+      <c r="M14" s="27" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="12" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>55</v>
       </c>
@@ -4662,12 +4800,18 @@
       <c r="I15" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="27"/>
-    </row>
-    <row r="16" spans="1:13" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="J15" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="K15" s="51" t="s">
+        <v>435</v>
+      </c>
+      <c r="L15" s="32"/>
+      <c r="M15" s="27" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="12" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
         <v>58</v>
       </c>
@@ -4694,11 +4838,13 @@
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="34"/>
+      <c r="K16" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="32"/>
       <c r="M16" s="27"/>
     </row>
-    <row r="17" spans="1:13" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="12" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
         <v>62</v>
       </c>
@@ -4725,11 +4871,13 @@
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="34"/>
+      <c r="K17" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="32"/>
       <c r="M17" s="27"/>
     </row>
-    <row r="18" spans="1:13" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="12" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>65</v>
       </c>
@@ -4756,11 +4904,13 @@
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="34"/>
+      <c r="K18" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="32"/>
       <c r="M18" s="27"/>
     </row>
-    <row r="19" spans="1:13" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="12" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
         <v>70</v>
       </c>
@@ -4785,11 +4935,13 @@
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="34"/>
+      <c r="K19" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="32"/>
       <c r="M19" s="27"/>
     </row>
-    <row r="20" spans="1:13" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="12" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
         <v>74</v>
       </c>
@@ -4814,11 +4966,13 @@
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="34"/>
+      <c r="K20" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L20" s="32"/>
       <c r="M20" s="27"/>
     </row>
-    <row r="21" spans="1:13" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="12" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
         <v>78</v>
       </c>
@@ -4843,11 +4997,13 @@
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="34"/>
+      <c r="K21" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="32"/>
       <c r="M21" s="27"/>
     </row>
-    <row r="22" spans="1:13" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="12" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
         <v>82</v>
       </c>
@@ -4872,11 +5028,13 @@
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="K22" s="51" t="s">
+        <v>23</v>
+      </c>
       <c r="L22" s="27"/>
       <c r="M22" s="27"/>
     </row>
-    <row r="23" spans="1:13" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="12" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
         <v>86</v>
       </c>
@@ -4901,11 +5059,13 @@
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="34"/>
+      <c r="K23" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L23" s="32"/>
       <c r="M23" s="27"/>
     </row>
-    <row r="24" spans="1:13" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="12" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
         <v>90</v>
       </c>
@@ -4930,11 +5090,13 @@
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="34"/>
+      <c r="K24" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L24" s="32"/>
       <c r="M24" s="27"/>
     </row>
-    <row r="25" spans="1:13" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="12" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
         <v>94</v>
       </c>
@@ -4959,11 +5121,13 @@
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+      <c r="K25" s="51" t="s">
+        <v>23</v>
+      </c>
       <c r="L25" s="27"/>
       <c r="M25" s="27"/>
     </row>
-    <row r="26" spans="1:13" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="12" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
         <v>98</v>
       </c>
@@ -4988,11 +5152,13 @@
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
+      <c r="K26" s="51" t="s">
+        <v>23</v>
+      </c>
       <c r="L26" s="27"/>
       <c r="M26" s="27"/>
     </row>
-    <row r="27" spans="1:13" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="12" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
         <v>102</v>
       </c>
@@ -5017,11 +5183,13 @@
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="34"/>
+      <c r="K27" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L27" s="32"/>
       <c r="M27" s="27"/>
     </row>
-    <row r="28" spans="1:13" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="12" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
         <v>106</v>
       </c>
@@ -5046,11 +5214,13 @@
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="34"/>
+      <c r="K28" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L28" s="32"/>
       <c r="M28" s="27"/>
     </row>
-    <row r="29" spans="1:13" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="12" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
         <v>110</v>
       </c>
@@ -5077,11 +5247,13 @@
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="34"/>
+      <c r="K29" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" s="32"/>
       <c r="M29" s="27"/>
     </row>
-    <row r="30" spans="1:13" s="12" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="12" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
         <v>115</v>
       </c>
@@ -5108,11 +5280,13 @@
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
+      <c r="K30" s="51" t="s">
+        <v>23</v>
+      </c>
       <c r="L30" s="27"/>
       <c r="M30" s="27"/>
     </row>
-    <row r="31" spans="1:13" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="12" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A31" s="26" t="s">
         <v>119</v>
       </c>
@@ -5139,11 +5313,13 @@
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
+      <c r="K31" s="51" t="s">
+        <v>23</v>
+      </c>
       <c r="L31" s="27"/>
       <c r="M31" s="27"/>
     </row>
-    <row r="32" spans="1:13" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="12" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A32" s="26" t="s">
         <v>123</v>
       </c>
@@ -5168,13 +5344,15 @@
       <c r="H32" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I32" s="6"/>
+      <c r="I32" s="53"/>
       <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
+      <c r="K32" s="51" t="s">
+        <v>23</v>
+      </c>
       <c r="L32" s="27"/>
       <c r="M32" s="27"/>
     </row>
-    <row r="33" spans="1:14" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" s="12" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A33" s="26" t="s">
         <v>127</v>
       </c>
@@ -5202,12 +5380,18 @@
       <c r="I33" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="J33" s="6"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="27"/>
-    </row>
-    <row r="34" spans="1:14" s="12" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="J33" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="K33" s="51" t="s">
+        <v>435</v>
+      </c>
+      <c r="L33" s="32"/>
+      <c r="M33" s="27" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="12" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A34" s="26" t="s">
         <v>132</v>
       </c>
@@ -5234,11 +5418,13 @@
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="34"/>
+      <c r="K34" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L34" s="32"/>
       <c r="M34" s="27"/>
     </row>
-    <row r="35" spans="1:14" s="12" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="12" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A35" s="26" t="s">
         <v>137</v>
       </c>
@@ -5263,11 +5449,13 @@
       </c>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
+      <c r="K35" s="51" t="s">
+        <v>23</v>
+      </c>
       <c r="L35" s="27"/>
       <c r="M35" s="27"/>
     </row>
-    <row r="36" spans="1:14" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" s="12" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
         <v>141</v>
       </c>
@@ -5292,11 +5480,13 @@
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
+      <c r="K36" s="51" t="s">
+        <v>23</v>
+      </c>
       <c r="L36" s="27"/>
       <c r="M36" s="27"/>
     </row>
-    <row r="37" spans="1:14" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="12" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
         <v>145</v>
       </c>
@@ -5321,11 +5511,13 @@
       </c>
       <c r="I37" s="21"/>
       <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
+      <c r="K37" s="51" t="s">
+        <v>23</v>
+      </c>
       <c r="L37" s="29"/>
       <c r="M37" s="29"/>
     </row>
-    <row r="38" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -5341,7 +5533,7 @@
       <c r="M38"/>
       <c r="N38"/>
     </row>
-    <row r="39" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -5357,7 +5549,7 @@
       <c r="M39"/>
       <c r="N39"/>
     </row>
-    <row r="40" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40"/>
       <c r="C40"/>
@@ -5373,7 +5565,7 @@
       <c r="M40"/>
       <c r="N40"/>
     </row>
-    <row r="41" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41"/>
       <c r="C41"/>
@@ -5389,7 +5581,7 @@
       <c r="M41"/>
       <c r="N41"/>
     </row>
-    <row r="42" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -5405,7 +5597,7 @@
       <c r="M42"/>
       <c r="N42"/>
     </row>
-    <row r="43" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -5421,7 +5613,7 @@
       <c r="M43"/>
       <c r="N43"/>
     </row>
-    <row r="45" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -5437,7 +5629,7 @@
       <c r="M45"/>
       <c r="N45"/>
     </row>
-    <row r="46" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46"/>
       <c r="C46"/>
@@ -5453,7 +5645,7 @@
       <c r="M46"/>
       <c r="N46"/>
     </row>
-    <row r="47" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -5469,7 +5661,7 @@
       <c r="M47"/>
       <c r="N47"/>
     </row>
-    <row r="48" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48"/>
       <c r="C48"/>
@@ -5485,7 +5677,7 @@
       <c r="M48"/>
       <c r="N48"/>
     </row>
-    <row r="49" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49"/>
       <c r="C49"/>
@@ -5501,7 +5693,7 @@
       <c r="M49"/>
       <c r="N49"/>
     </row>
-    <row r="50" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50"/>
       <c r="C50"/>
@@ -5517,7 +5709,7 @@
       <c r="M50"/>
       <c r="N50"/>
     </row>
-    <row r="51" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51"/>
       <c r="C51"/>
@@ -5533,7 +5725,7 @@
       <c r="M51"/>
       <c r="N51"/>
     </row>
-    <row r="52" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52"/>
       <c r="C52"/>
@@ -5549,7 +5741,7 @@
       <c r="M52"/>
       <c r="N52"/>
     </row>
-    <row r="53" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53"/>
       <c r="C53"/>
@@ -5565,7 +5757,7 @@
       <c r="M53"/>
       <c r="N53"/>
     </row>
-    <row r="54" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54"/>
       <c r="C54"/>
@@ -5581,7 +5773,7 @@
       <c r="M54"/>
       <c r="N54"/>
     </row>
-    <row r="55" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55"/>
       <c r="C55"/>
@@ -5597,7 +5789,7 @@
       <c r="M55"/>
       <c r="N55"/>
     </row>
-    <row r="56" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56"/>
       <c r="C56"/>
@@ -5613,7 +5805,7 @@
       <c r="M56"/>
       <c r="N56"/>
     </row>
-    <row r="57" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57"/>
       <c r="C57"/>
@@ -5629,7 +5821,7 @@
       <c r="M57"/>
       <c r="N57"/>
     </row>
-    <row r="58" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -5645,7 +5837,7 @@
       <c r="M58"/>
       <c r="N58"/>
     </row>
-    <row r="59" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -5661,7 +5853,7 @@
       <c r="M59"/>
       <c r="N59"/>
     </row>
-    <row r="60" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -5677,7 +5869,7 @@
       <c r="M60"/>
       <c r="N60"/>
     </row>
-    <row r="61" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61"/>
       <c r="C61"/>
@@ -5693,7 +5885,7 @@
       <c r="M61"/>
       <c r="N61"/>
     </row>
-    <row r="62" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62"/>
       <c r="C62"/>
@@ -5709,7 +5901,7 @@
       <c r="M62"/>
       <c r="N62"/>
     </row>
-    <row r="63" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -5725,7 +5917,7 @@
       <c r="M63"/>
       <c r="N63"/>
     </row>
-    <row r="64" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64"/>
       <c r="C64"/>
@@ -5741,7 +5933,7 @@
       <c r="M64"/>
       <c r="N64"/>
     </row>
-    <row r="65" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65"/>
       <c r="C65"/>
@@ -5757,7 +5949,7 @@
       <c r="M65"/>
       <c r="N65"/>
     </row>
-    <row r="66" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66"/>
       <c r="C66"/>
@@ -5773,7 +5965,7 @@
       <c r="M66"/>
       <c r="N66"/>
     </row>
-    <row r="67" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67"/>
       <c r="C67"/>
@@ -5789,7 +5981,7 @@
       <c r="M67"/>
       <c r="N67"/>
     </row>
-    <row r="68" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68"/>
       <c r="C68"/>
@@ -5805,7 +5997,7 @@
       <c r="M68"/>
       <c r="N68"/>
     </row>
-    <row r="69" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69"/>
       <c r="C69"/>
@@ -5821,7 +6013,7 @@
       <c r="M69"/>
       <c r="N69"/>
     </row>
-    <row r="70" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70"/>
       <c r="C70"/>
@@ -5837,7 +6029,7 @@
       <c r="M70"/>
       <c r="N70"/>
     </row>
-    <row r="71" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71"/>
       <c r="C71"/>
@@ -5853,7 +6045,7 @@
       <c r="M71"/>
       <c r="N71"/>
     </row>
-    <row r="72" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72"/>
       <c r="C72"/>
@@ -5869,7 +6061,7 @@
       <c r="M72"/>
       <c r="N72"/>
     </row>
-    <row r="73" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73"/>
       <c r="C73"/>
@@ -5885,7 +6077,7 @@
       <c r="M73"/>
       <c r="N73"/>
     </row>
-    <row r="74" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74"/>
       <c r="C74"/>
@@ -5901,7 +6093,7 @@
       <c r="M74"/>
       <c r="N74"/>
     </row>
-    <row r="75" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75"/>
       <c r="C75"/>
@@ -5917,7 +6109,7 @@
       <c r="M75"/>
       <c r="N75"/>
     </row>
-    <row r="76" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76"/>
       <c r="C76"/>
@@ -5933,7 +6125,7 @@
       <c r="M76"/>
       <c r="N76"/>
     </row>
-    <row r="77" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77"/>
       <c r="C77"/>
@@ -5949,7 +6141,7 @@
       <c r="M77"/>
       <c r="N77"/>
     </row>
-    <row r="78" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78"/>
       <c r="C78"/>
@@ -5965,7 +6157,7 @@
       <c r="M78"/>
       <c r="N78"/>
     </row>
-    <row r="79" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79"/>
       <c r="C79"/>
@@ -5981,7 +6173,7 @@
       <c r="M79"/>
       <c r="N79"/>
     </row>
-    <row r="80" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80"/>
       <c r="C80"/>
@@ -5997,7 +6189,7 @@
       <c r="M80"/>
       <c r="N80"/>
     </row>
-    <row r="81" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81"/>
       <c r="C81"/>
@@ -6013,7 +6205,7 @@
       <c r="M81"/>
       <c r="N81"/>
     </row>
-    <row r="82" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82"/>
       <c r="C82"/>
@@ -6029,7 +6221,7 @@
       <c r="M82"/>
       <c r="N82"/>
     </row>
-    <row r="83" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83"/>
       <c r="C83"/>
@@ -6045,7 +6237,7 @@
       <c r="M83"/>
       <c r="N83"/>
     </row>
-    <row r="84" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84"/>
       <c r="C84"/>
@@ -6061,7 +6253,7 @@
       <c r="M84"/>
       <c r="N84"/>
     </row>
-    <row r="85" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85"/>
       <c r="C85"/>
@@ -6077,7 +6269,7 @@
       <c r="M85"/>
       <c r="N85"/>
     </row>
-    <row r="86" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86"/>
       <c r="C86"/>
@@ -6093,7 +6285,7 @@
       <c r="M86"/>
       <c r="N86"/>
     </row>
-    <row r="87" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87"/>
       <c r="C87"/>
@@ -6109,7 +6301,7 @@
       <c r="M87"/>
       <c r="N87"/>
     </row>
-    <row r="88" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88"/>
       <c r="C88"/>
@@ -6125,7 +6317,7 @@
       <c r="M88"/>
       <c r="N88"/>
     </row>
-    <row r="89" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89"/>
       <c r="C89"/>
@@ -6141,7 +6333,7 @@
       <c r="M89"/>
       <c r="N89"/>
     </row>
-    <row r="90" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90"/>
       <c r="C90"/>
@@ -6157,7 +6349,7 @@
       <c r="M90"/>
       <c r="N90"/>
     </row>
-    <row r="91" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91"/>
       <c r="C91"/>
@@ -6173,7 +6365,7 @@
       <c r="M91"/>
       <c r="N91"/>
     </row>
-    <row r="92" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92"/>
       <c r="C92"/>
@@ -6189,7 +6381,7 @@
       <c r="M92"/>
       <c r="N92"/>
     </row>
-    <row r="93" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93"/>
       <c r="C93"/>
@@ -6205,7 +6397,7 @@
       <c r="M93"/>
       <c r="N93"/>
     </row>
-    <row r="94" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94"/>
       <c r="C94"/>
@@ -6221,7 +6413,7 @@
       <c r="M94"/>
       <c r="N94"/>
     </row>
-    <row r="95" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95"/>
       <c r="C95"/>
@@ -6237,7 +6429,7 @@
       <c r="M95"/>
       <c r="N95"/>
     </row>
-    <row r="96" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96"/>
       <c r="C96"/>
@@ -6253,7 +6445,7 @@
       <c r="M96"/>
       <c r="N96"/>
     </row>
-    <row r="97" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97"/>
       <c r="C97"/>
@@ -6269,7 +6461,7 @@
       <c r="M97"/>
       <c r="N97"/>
     </row>
-    <row r="98" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98"/>
       <c r="C98"/>
@@ -6285,7 +6477,7 @@
       <c r="M98"/>
       <c r="N98"/>
     </row>
-    <row r="99" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99"/>
       <c r="C99"/>
@@ -6301,7 +6493,7 @@
       <c r="M99"/>
       <c r="N99"/>
     </row>
-    <row r="100" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100"/>
       <c r="C100"/>
@@ -6317,7 +6509,7 @@
       <c r="M100"/>
       <c r="N100"/>
     </row>
-    <row r="101" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101"/>
       <c r="C101"/>
@@ -6333,7 +6525,7 @@
       <c r="M101"/>
       <c r="N101"/>
     </row>
-    <row r="102" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102"/>
       <c r="C102"/>
@@ -6349,7 +6541,7 @@
       <c r="M102"/>
       <c r="N102"/>
     </row>
-    <row r="103" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103"/>
       <c r="C103"/>
@@ -6370,22 +6562,30 @@
     <mergeCell ref="B1:E2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="K6:L21 K23:L24 K27:L29 K33:L34">
-    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="FAIL">
+  <conditionalFormatting sqref="K6:L16 L23:L24 L27:L29 K33:L34 L17:L21 K17:K32">
+    <cfRule type="containsText" dxfId="18" priority="7" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",K6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",K6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6:M37">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="16" priority="6">
       <formula>LEN(M6) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I15">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>LEN(I6) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K35:K37">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",K35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6400,44 +6600,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B325D8-3CF6-4073-AC79-DF4037A6AAE2}">
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+    <sheetView topLeftCell="C58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" customWidth="1"/>
     <col min="8" max="8" width="37" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.85546875" customWidth="1"/>
-    <col min="11" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.88671875" customWidth="1"/>
+    <col min="11" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="39" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="41"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-    </row>
-    <row r="5" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="42"/>
+    </row>
+    <row r="5" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
@@ -6471,14 +6671,14 @@
       <c r="K5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="33" t="s">
+      <c r="L5" s="5" t="s">
         <v>150</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>151</v>
       </c>
@@ -6508,10 +6708,10 @@
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="11"/>
-      <c r="L6" s="36"/>
+      <c r="L6" s="34"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>153</v>
       </c>
@@ -6544,7 +6744,7 @@
       <c r="L7" s="22"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>154</v>
       </c>
@@ -6577,7 +6777,7 @@
       <c r="L8" s="22"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>155</v>
       </c>
@@ -6610,7 +6810,7 @@
       <c r="L9" s="22"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>156</v>
       </c>
@@ -6643,7 +6843,7 @@
       <c r="L10" s="22"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>157</v>
       </c>
@@ -6676,7 +6876,7 @@
       <c r="L11" s="22"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>158</v>
       </c>
@@ -6709,7 +6909,7 @@
       <c r="L12" s="22"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>159</v>
       </c>
@@ -6742,7 +6942,7 @@
       <c r="L13" s="22"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:13" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="12" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>160</v>
       </c>
@@ -6775,7 +6975,7 @@
       <c r="L14" s="22"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:13" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="12" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>161</v>
       </c>
@@ -6808,7 +7008,7 @@
       <c r="L15" s="22"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:13" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="12" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>162</v>
       </c>
@@ -6839,7 +7039,7 @@
       <c r="L16" s="22"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:13" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="12" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>163</v>
       </c>
@@ -6870,7 +7070,7 @@
       <c r="L17" s="22"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:13" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="12" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>164</v>
       </c>
@@ -6903,7 +7103,7 @@
       <c r="L18" s="22"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="1:13" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>165</v>
       </c>
@@ -6932,7 +7132,7 @@
       <c r="L19" s="22"/>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="1:13" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>166</v>
       </c>
@@ -6961,7 +7161,7 @@
       <c r="L20" s="22"/>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="1:13" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>167</v>
       </c>
@@ -6990,7 +7190,7 @@
       <c r="L21" s="22"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>168</v>
       </c>
@@ -7021,7 +7221,7 @@
       <c r="L22" s="22"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>169</v>
       </c>
@@ -7052,7 +7252,7 @@
       <c r="L23" s="22"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>170</v>
       </c>
@@ -7083,7 +7283,7 @@
       <c r="L24" s="22"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>171</v>
       </c>
@@ -7114,7 +7314,7 @@
       <c r="L25" s="22"/>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>172</v>
       </c>
@@ -7145,7 +7345,7 @@
       <c r="L26" s="22"/>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>173</v>
       </c>
@@ -7176,7 +7376,7 @@
       <c r="L27" s="22"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="1:13" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>174</v>
       </c>
@@ -7207,7 +7407,7 @@
       <c r="L28" s="22"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="12" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>175</v>
       </c>
@@ -7238,7 +7438,7 @@
       <c r="L29" s="22"/>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="1:13" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="12" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>176</v>
       </c>
@@ -7269,7 +7469,7 @@
       <c r="L30" s="22"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="1:13" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="12" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>177</v>
       </c>
@@ -7300,7 +7500,7 @@
       <c r="L31" s="22"/>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="1:13" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="12" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>178</v>
       </c>
@@ -7331,7 +7531,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="6"/>
     </row>
-    <row r="33" spans="1:13" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="12" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>179</v>
       </c>
@@ -7362,7 +7562,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="1:13" s="12" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="12" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>180</v>
       </c>
@@ -7393,7 +7593,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="1:13" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="12" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>181</v>
       </c>
@@ -7422,7 +7622,7 @@
       <c r="L35" s="22"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="1:13" s="12" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="12" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>182</v>
       </c>
@@ -7451,7 +7651,7 @@
       <c r="L36" s="22"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="1:13" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="12" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>183</v>
       </c>
@@ -7480,7 +7680,7 @@
       <c r="L37" s="24"/>
       <c r="M37" s="21"/>
     </row>
-    <row r="38" spans="1:13" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -7495,21 +7695,21 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="1:13" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="39" t="s">
+    <row r="39" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="41"/>
-    </row>
-    <row r="40" spans="1:13" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="42"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="44"/>
-    </row>
-    <row r="42" spans="1:13" ht="39" x14ac:dyDescent="0.25">
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="39"/>
+    </row>
+    <row r="40" spans="1:13" ht="25.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="40"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="42"/>
+    </row>
+    <row r="42" spans="1:13" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
         <v>1</v>
       </c>
@@ -7543,14 +7743,14 @@
       <c r="K42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L42" s="33" t="s">
+      <c r="L42" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="M42" s="33" t="s">
+      <c r="M42" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="225" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A43" s="23" t="s">
         <v>185</v>
       </c>
@@ -7584,10 +7784,10 @@
       <c r="K43" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="L43" s="36"/>
-      <c r="M43" s="36"/>
-    </row>
-    <row r="44" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+      <c r="L43" s="34"/>
+      <c r="M43" s="34"/>
+    </row>
+    <row r="44" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A44" s="23" t="s">
         <v>191</v>
       </c>
@@ -7624,7 +7824,7 @@
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
     </row>
-    <row r="45" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A45" s="23" t="s">
         <v>194</v>
       </c>
@@ -7661,7 +7861,7 @@
       <c r="L45" s="22"/>
       <c r="M45" s="22"/>
     </row>
-    <row r="46" spans="1:13" ht="225" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
         <v>197</v>
       </c>
@@ -7698,7 +7898,7 @@
       <c r="L46" s="22"/>
       <c r="M46" s="22"/>
     </row>
-    <row r="47" spans="1:13" ht="225" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A47" s="23" t="s">
         <v>200</v>
       </c>
@@ -7735,7 +7935,7 @@
       <c r="L47" s="22"/>
       <c r="M47" s="22"/>
     </row>
-    <row r="48" spans="1:13" ht="225" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A48" s="23" t="s">
         <v>204</v>
       </c>
@@ -7772,7 +7972,7 @@
       <c r="L48" s="22"/>
       <c r="M48" s="22"/>
     </row>
-    <row r="49" spans="1:13" ht="255" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="216" x14ac:dyDescent="0.3">
       <c r="A49" s="23" t="s">
         <v>207</v>
       </c>
@@ -7809,7 +8009,7 @@
       <c r="L49" s="22"/>
       <c r="M49" s="22"/>
     </row>
-    <row r="50" spans="1:13" ht="285" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A50" s="23" t="s">
         <v>212</v>
       </c>
@@ -7846,7 +8046,7 @@
       <c r="L50" s="22"/>
       <c r="M50" s="22"/>
     </row>
-    <row r="51" spans="1:13" ht="285" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A51" s="23" t="s">
         <v>216</v>
       </c>
@@ -7883,7 +8083,7 @@
       <c r="L51" s="22"/>
       <c r="M51" s="22"/>
     </row>
-    <row r="52" spans="1:13" ht="225" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A52" s="23" t="s">
         <v>219</v>
       </c>
@@ -7920,7 +8120,7 @@
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
     </row>
-    <row r="53" spans="1:13" ht="240" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A53" s="23" t="s">
         <v>222</v>
       </c>
@@ -7957,7 +8157,7 @@
       <c r="L53" s="22"/>
       <c r="M53" s="22"/>
     </row>
-    <row r="54" spans="1:13" ht="240" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A54" s="23" t="s">
         <v>226</v>
       </c>
@@ -7994,7 +8194,7 @@
       <c r="L54" s="22"/>
       <c r="M54" s="22"/>
     </row>
-    <row r="55" spans="1:13" ht="316.89999999999998" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="316.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="23" t="s">
         <v>229</v>
       </c>
@@ -8031,7 +8231,7 @@
       <c r="L55" s="22"/>
       <c r="M55" s="22"/>
     </row>
-    <row r="56" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A56" s="23" t="s">
         <v>232</v>
       </c>
@@ -8068,7 +8268,7 @@
       <c r="L56" s="22"/>
       <c r="M56" s="22"/>
     </row>
-    <row r="57" spans="1:13" ht="240" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="216" x14ac:dyDescent="0.3">
       <c r="A57" s="23" t="s">
         <v>237</v>
       </c>
@@ -8105,7 +8305,7 @@
       <c r="L57" s="22"/>
       <c r="M57" s="22"/>
     </row>
-    <row r="58" spans="1:13" ht="225" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A58" s="23" t="s">
         <v>243</v>
       </c>
@@ -8142,7 +8342,7 @@
       <c r="L58" s="22"/>
       <c r="M58" s="22"/>
     </row>
-    <row r="59" spans="1:13" ht="240" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A59" s="23" t="s">
         <v>247</v>
       </c>
@@ -8179,7 +8379,7 @@
       <c r="L59" s="22"/>
       <c r="M59" s="22"/>
     </row>
-    <row r="60" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A60" s="23" t="s">
         <v>251</v>
       </c>
@@ -8216,7 +8416,7 @@
       <c r="L60" s="22"/>
       <c r="M60" s="22"/>
     </row>
-    <row r="61" spans="1:13" ht="225" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A61" s="23" t="s">
         <v>255</v>
       </c>
@@ -8253,7 +8453,7 @@
       <c r="L61" s="22"/>
       <c r="M61" s="22"/>
     </row>
-    <row r="62" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A62" s="23" t="s">
         <v>259</v>
       </c>
@@ -8290,7 +8490,7 @@
       <c r="L62" s="22"/>
       <c r="M62" s="22"/>
     </row>
-    <row r="63" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A63" s="23" t="s">
         <v>263</v>
       </c>
@@ -8327,7 +8527,7 @@
       <c r="L63" s="22"/>
       <c r="M63" s="22"/>
     </row>
-    <row r="64" spans="1:13" ht="286.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="286.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="23" t="s">
         <v>266</v>
       </c>
@@ -8371,33 +8571,33 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="K6:K21 K23:K24 K27:K29 K33:K34">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",K6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",K6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K50:K64">
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",K50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",K50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I15">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>LEN(I6) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>LEN(I18) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:I28">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>LEN(I22) = 0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8412,44 +8612,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12FB3170-0DBB-443D-96A1-2095AFA2B236}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="43" t="s">
         <v>271</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="50"/>
-    </row>
-    <row r="4" spans="1:13" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45"/>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
+    </row>
+    <row r="4" spans="1:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -8483,14 +8683,14 @@
       <c r="K4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="L4" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="M4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>273</v>
       </c>
@@ -8516,10 +8716,10 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="11"/>
-      <c r="L5" s="32"/>
+      <c r="L5" s="31"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>278</v>
       </c>
@@ -8548,7 +8748,7 @@
       <c r="L6" s="19"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>281</v>
       </c>
@@ -8581,7 +8781,7 @@
       </c>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>285</v>
       </c>
@@ -8610,7 +8810,7 @@
       <c r="L8" s="19"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>288</v>
       </c>
@@ -8639,7 +8839,7 @@
       <c r="L9" s="19"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>291</v>
       </c>
@@ -8668,7 +8868,7 @@
       <c r="L10" s="19"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>294</v>
       </c>
@@ -8697,7 +8897,7 @@
       <c r="L11" s="19"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>297</v>
       </c>
@@ -8726,7 +8926,7 @@
       <c r="L12" s="19"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>300</v>
       </c>
@@ -8755,7 +8955,7 @@
       <c r="L13" s="19"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>303</v>
       </c>
@@ -8784,7 +8984,7 @@
       <c r="L14" s="19"/>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="1:13" ht="91.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>306</v>
       </c>
@@ -8813,7 +9013,7 @@
       <c r="L15" s="19"/>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>310</v>
       </c>
@@ -8842,7 +9042,7 @@
       <c r="L16" s="19"/>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>313</v>
       </c>
@@ -8871,59 +9071,55 @@
       <c r="L17" s="19"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="20" spans="1:13" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="50" t="s">
         <v>392</v>
       </c>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="31"/>
-    </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+    </row>
+    <row r="23" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
         <v>387</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="49" t="s">
         <v>388</v>
       </c>
-      <c r="C23" s="51"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C23" s="49"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="30"/>
       <c r="B24" s="30"/>
       <c r="C24" s="30"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="51" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="49" t="s">
         <v>389</v>
       </c>
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="49" t="s">
         <v>390</v>
       </c>
-      <c r="C25" s="51"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="51"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="51"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M30" s="31"/>
+      <c r="C25" s="49"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -8956,39 +9152,39 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="9" width="28.42578125" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
+    <col min="8" max="9" width="28.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="43" t="s">
         <v>316</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="50"/>
-    </row>
-    <row r="4" spans="1:13" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45"/>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
+    </row>
+    <row r="4" spans="1:13" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -9029,7 +9225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>317</v>
       </c>
@@ -9058,7 +9254,7 @@
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
     </row>
-    <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>322</v>
       </c>
@@ -9087,7 +9283,7 @@
       <c r="L6" s="19"/>
       <c r="M6" s="19"/>
     </row>
-    <row r="7" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>325</v>
       </c>
@@ -9116,7 +9312,7 @@
       <c r="L7" s="19"/>
       <c r="M7" s="19"/>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>328</v>
       </c>
@@ -9145,7 +9341,7 @@
       <c r="L8" s="19"/>
       <c r="M8" s="19"/>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>331</v>
       </c>
@@ -9174,7 +9370,7 @@
       <c r="L9" s="19"/>
       <c r="M9" s="19"/>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>334</v>
       </c>
@@ -9203,7 +9399,7 @@
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>337</v>
       </c>
@@ -9232,7 +9428,7 @@
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>340</v>
       </c>
@@ -9261,7 +9457,7 @@
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>343</v>
       </c>
@@ -9290,7 +9486,7 @@
       <c r="L13" s="19"/>
       <c r="M13" s="19"/>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>346</v>
       </c>
@@ -9319,7 +9515,7 @@
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
     </row>
-    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>349</v>
       </c>
@@ -9348,7 +9544,7 @@
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>352</v>
       </c>
@@ -9377,7 +9573,7 @@
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
     </row>
-    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>355</v>
       </c>
@@ -9406,7 +9602,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
     </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>358</v>
       </c>
@@ -9435,7 +9631,7 @@
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
     </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>361</v>
       </c>

</xml_diff>